<commit_message>
Update flow property info
</commit_message>
<xml_diff>
--- a/jupyter/PSM-hackathon-leaf-flows_annotated.xlsx
+++ b/jupyter/PSM-hackathon-leaf-flows_annotated.xlsx
@@ -5,14 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="flow" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="quantity" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="terminations" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="mass_hints" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">flow!$A$1:$L$811</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Criteria" vbProcedure="false">flow!$C$1:$C$810</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6114" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6272" uniqueCount="1100">
   <si>
     <t xml:space="preserve">external_ref</t>
   </si>
@@ -3300,6 +3303,30 @@
   </si>
   <si>
     <t xml:space="preserve">Number of items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USLCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USEEIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EI34APOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fd5bb172-5a3b-4b51-aa54-9013d76cbd2d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price</t>
   </si>
 </sst>
 </file>
@@ -3396,21 +3423,17 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L811"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3419,7 +3442,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -25844,7 +25867,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L811"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -25852,7 +25874,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -25863,7 +25884,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -25913,4 +25934,1002 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F54"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>748</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>567</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>978</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I46"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>748</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>978</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>850</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>635</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>984</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>993</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Terminations-- USLCI and USEEIO
</commit_message>
<xml_diff>
--- a/jupyter/PSM-hackathon-leaf-flows_annotated.xlsx
+++ b/jupyter/PSM-hackathon-leaf-flows_annotated.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="flow" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6272" uniqueCount="1100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6378" uniqueCount="1143">
   <si>
     <t xml:space="preserve">external_ref</t>
   </si>
@@ -3317,7 +3317,136 @@
     <t xml:space="preserve">ELCD</t>
   </si>
   <si>
+    <t xml:space="preserve">a2e7aa17-9318-3bb8-91d6-22a32a9e8019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ad81ce2a-e3c5-3695-a2ef-812cd8b79dd3</t>
+  </si>
+  <si>
     <t xml:space="preserve">fd5bb172-5a3b-4b51-aa54-9013d76cbd2d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f61ecd3b-fdba-3739-8051-1d4bb0c2d98e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adaf0129-e55e-36e7-b2a1-d2b41f1fff11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77fe2197-8861-3569-8d85-07151789b1e7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2b196386-eb1a-352a-aeda-4d003144f6df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40ef9b2b-baaa-37b5-8dd9-185a23a0c9e0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">076898a5-e1ce-3c50-9df4-6445fc0bb6aa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49f5324b-fc33-36e9-b5af-3c80d73492bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">265a41f3-c5ef-3e6e-a7db-d7592121bc12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f071aaba-fe95-37fd-a226-53c60fe29376</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41ecdfe1-8026-3373-96c4-ee1921f2525c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d7553a09-54db-3bf0-aa06-a68819dab715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5d274fc8-65f3-3f3a-a583-f12cace7c494</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230e8d51-1f4d-3459-be47-429b0b828add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fcdc8a7a-b10b-34bd-8ab3-65155dd4a762</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4edd87d7-666f-3226-a10c-a7b32d46f2fc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88b44b36-2322-39a8-9c54-6b89b1b43cd4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cf1241fd-8c01-3412-9030-8650b8e75669</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84d335bb-f2ce-38dc-b81f-55d4eb7408c7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">555ec871-5359-34e8-90d5-d2fc6b0cb5dd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c18fe11e-9890-3e41-a2a6-36198c86cea5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1ba8424c-2bdb-353e-8ea4-5e8d3bd477b8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cb881099-7dd3-31ab-888f-555cccb34622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">874dc726-50f1-300b-958f-9335fd1c53cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">031048f1-8668-3af1-a8be-b329cd80e6b6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a76535b9-f6de-306b-a043-3ec2846df5c6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09652625-aaa5-36bd-a2fb-0d05a3863571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ce38752e-c414-3175-9482-ce663a909a0c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7b69255a-a7b2-318e-9433-54b7c4d13ece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e10de570-42e6-3cb6-98fe-7bf6da57046c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0a075756-e4af-3da7-a521-c6f460e8470e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b19fe3da-392e-36af-9342-910be1d2160a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fa60e60f-73f0-3e20-bb3a-073e4a9469cc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">406f2854-27c5-3871-a9d5-80d29a4a39eb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a6cedcb1-f22c-3fc6-b6ee-7cb0c00da33d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c378e883-97fc-3714-b923-d7271b8fcbac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bc251c04-d2b2-366f-af0c-99d8fc2ed467</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7022c714-ec1a-3bec-ae9f-ed7769841d7c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c19569ac-f0ab-453a-b70b-43f73bad11f8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8560388b-7ea1-38b7-befc-fd25d5deb450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfd38ecd-840a-3b28-88d6-a382831c6d9c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ab2436bc-97db-3154-898e-2c49ca4b698e</t>
   </si>
   <si>
     <t xml:space="preserve">Keyword</t>
@@ -3433,7 +3562,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="1" sqref="D24 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25885,7 +26014,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D24 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25943,13 +26072,15 @@
   </sheetPr>
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="37.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="61.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.67"/>
   </cols>
   <sheetData>
@@ -25980,8 +26111,14 @@
       <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>1097</v>
+      </c>
       <c r="E2" s="0" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25991,6 +26128,12 @@
       <c r="B3" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>1100</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -25999,6 +26142,12 @@
       <c r="B4" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C4" s="0" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>1100</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -26007,11 +26156,23 @@
       <c r="B5" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="C5" s="0" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>1103</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="C6" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>1105</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -26020,6 +26181,12 @@
       <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="C7" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>1106</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -26028,6 +26195,12 @@
       <c r="B8" s="0" t="s">
         <v>337</v>
       </c>
+      <c r="C8" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>1107</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -26036,6 +26209,12 @@
       <c r="B9" s="0" t="s">
         <v>850</v>
       </c>
+      <c r="C9" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>1105</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -26043,6 +26222,12 @@
       </c>
       <c r="B10" s="1" t="s">
         <v>854</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>1109</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26052,6 +26237,12 @@
       <c r="B11" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="C11" s="0" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>1097</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -26060,6 +26251,12 @@
       <c r="B12" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="C12" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>1112</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -26068,6 +26265,12 @@
       <c r="B13" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="C13" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>1113</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -26076,6 +26279,12 @@
       <c r="B14" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="C14" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>1103</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -26084,6 +26293,12 @@
       <c r="B15" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="C15" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>1103</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -26092,6 +26307,12 @@
       <c r="B16" s="0" t="s">
         <v>37</v>
       </c>
+      <c r="C16" s="0" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>1113</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -26100,6 +26321,12 @@
       <c r="B17" s="0" t="s">
         <v>260</v>
       </c>
+      <c r="C17" s="0" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>1117</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -26108,6 +26335,12 @@
       <c r="B18" s="0" t="s">
         <v>285</v>
       </c>
+      <c r="C18" s="0" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>1118</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -26116,6 +26349,12 @@
       <c r="B19" s="0" t="s">
         <v>294</v>
       </c>
+      <c r="C19" s="0" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -26124,6 +26363,12 @@
       <c r="B20" s="0" t="s">
         <v>302</v>
       </c>
+      <c r="C20" s="0" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>1122</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -26132,6 +26377,12 @@
       <c r="B21" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="C21" s="0" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>1117</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -26140,6 +26391,12 @@
       <c r="B22" s="0" t="s">
         <v>349</v>
       </c>
+      <c r="C22" s="0" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>1123</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -26148,11 +26405,23 @@
       <c r="B23" s="0" t="s">
         <v>357</v>
       </c>
+      <c r="C23" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>1124</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="C24" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>1105</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
@@ -26161,6 +26430,12 @@
       <c r="B25" s="0" t="s">
         <v>635</v>
       </c>
+      <c r="C25" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>1124</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -26169,6 +26444,12 @@
       <c r="B26" s="1" t="s">
         <v>687</v>
       </c>
+      <c r="C26" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>1123</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -26177,6 +26458,12 @@
       <c r="B27" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="C27" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>1106</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -26185,6 +26472,12 @@
       <c r="B28" s="0" t="s">
         <v>984</v>
       </c>
+      <c r="C28" s="0" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>1118</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -26193,6 +26486,12 @@
       <c r="B29" s="0" t="s">
         <v>993</v>
       </c>
+      <c r="C29" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>1124</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -26201,6 +26500,12 @@
       <c r="B30" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="C30" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>1103</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
@@ -26209,6 +26514,12 @@
       <c r="B31" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="C31" s="0" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>1097</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -26217,6 +26528,12 @@
       <c r="B32" s="1" t="s">
         <v>377</v>
       </c>
+      <c r="C32" s="0" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
@@ -26225,11 +26542,23 @@
       <c r="B33" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="C33" s="0" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>1097</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>319</v>
       </c>
+      <c r="C34" s="0" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>1097</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -26238,6 +26567,12 @@
       <c r="B35" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C35" s="0" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>1097</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -26246,6 +26581,12 @@
       <c r="B36" s="0" t="s">
         <v>377</v>
       </c>
+      <c r="C36" s="0" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -26254,6 +26595,12 @@
       <c r="B37" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="C37" s="0" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>1097</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
@@ -26262,6 +26609,12 @@
       <c r="B38" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C38" s="0" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>1097</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
@@ -26270,6 +26623,12 @@
       <c r="B39" s="0" t="s">
         <v>377</v>
       </c>
+      <c r="C39" s="0" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
@@ -26278,6 +26637,12 @@
       <c r="B40" s="0" t="s">
         <v>377</v>
       </c>
+      <c r="C40" s="0" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
@@ -26286,6 +26651,12 @@
       <c r="B41" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="C41" s="0" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>1131</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -26294,6 +26665,12 @@
       <c r="B42" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="C42" s="0" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>1132</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
@@ -26302,6 +26679,12 @@
       <c r="B43" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="C43" s="0" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>1113</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -26310,6 +26693,12 @@
       <c r="B44" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="C44" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>1135</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -26318,6 +26707,12 @@
       <c r="B45" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="C45" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>1135</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -26326,6 +26721,12 @@
       <c r="B46" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="C46" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>1103</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -26334,6 +26735,12 @@
       <c r="B47" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="C47" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>1103</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
@@ -26342,6 +26749,12 @@
       <c r="B48" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="C48" s="0" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>1113</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
@@ -26350,6 +26763,12 @@
       <c r="B49" s="0" t="s">
         <v>854</v>
       </c>
+      <c r="C49" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>1109</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -26358,6 +26777,12 @@
       <c r="B50" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="C50" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>1113</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -26366,6 +26791,12 @@
       <c r="B51" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="C51" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>1103</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
@@ -26374,6 +26805,12 @@
       <c r="B52" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="C52" s="0" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>1135</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
@@ -26382,6 +26819,12 @@
       <c r="B53" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="C53" s="0" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
@@ -26389,6 +26832,12 @@
       </c>
       <c r="B54" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>1113</v>
       </c>
     </row>
   </sheetData>
@@ -26409,21 +26858,21 @@
   </sheetPr>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="D24 C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>1097</v>
+        <v>1140</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1098</v>
+        <v>1141</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1099</v>
+        <v>1142</v>
       </c>
       <c r="G1" s="1"/>
       <c r="I1" s="1"/>

</xml_diff>

<commit_message>
Simple product model to disclosure
</commit_message>
<xml_diff>
--- a/jupyter/PSM-hackathon-leaf-flows_annotated.xlsx
+++ b/jupyter/PSM-hackathon-leaf-flows_annotated.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6378" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6414" uniqueCount="1159">
   <si>
     <t xml:space="preserve">external_ref</t>
   </si>
@@ -3305,16 +3305,16 @@
     <t xml:space="preserve">Number of items</t>
   </si>
   <si>
-    <t xml:space="preserve">USLCI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USEEIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EI34APOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELCD</t>
+    <t xml:space="preserve">local.uslci.olca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">local.usepa.useeio.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">local.ecoinvent.3.4.apos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">local.elcd.3.2</t>
   </si>
   <si>
     <t xml:space="preserve">a2e7aa17-9318-3bb8-91d6-22a32a9e8019</t>
@@ -3326,21 +3326,33 @@
     <t xml:space="preserve">fd5bb172-5a3b-4b51-aa54-9013d76cbd2d</t>
   </si>
   <si>
+    <t xml:space="preserve">76d6aaa4-37e2-40b2-994c-03292b600074</t>
+  </si>
+  <si>
     <t xml:space="preserve">f61ecd3b-fdba-3739-8051-1d4bb0c2d98e</t>
   </si>
   <si>
     <t xml:space="preserve">adaf0129-e55e-36e7-b2a1-d2b41f1fff11</t>
   </si>
   <si>
+    <t xml:space="preserve">09215eb1-5fc9-11dd-ad8b-0800200c9a66</t>
+  </si>
+  <si>
     <t xml:space="preserve">77fe2197-8861-3569-8d85-07151789b1e7</t>
   </si>
   <si>
+    <t xml:space="preserve">09215eb0-5fc9-11dd-ad8b-0800200c9a66</t>
+  </si>
+  <si>
     <t xml:space="preserve">2b196386-eb1a-352a-aeda-4d003144f6df</t>
   </si>
   <si>
     <t xml:space="preserve">40ef9b2b-baaa-37b5-8dd9-185a23a0c9e0</t>
   </si>
   <si>
+    <t xml:space="preserve">268a11fb-baf2-4b9e-8867-38bea0e76ef6</t>
+  </si>
+  <si>
     <t xml:space="preserve">076898a5-e1ce-3c50-9df4-6445fc0bb6aa</t>
   </si>
   <si>
@@ -3359,18 +3371,30 @@
     <t xml:space="preserve">d7553a09-54db-3bf0-aa06-a68819dab715</t>
   </si>
   <si>
+    <t xml:space="preserve">e16174fe-6542-4572-90bc-8980616ebe53</t>
+  </si>
+  <si>
     <t xml:space="preserve">5d274fc8-65f3-3f3a-a583-f12cace7c494</t>
   </si>
   <si>
+    <t xml:space="preserve">4575c944-457d-4825-82ff-17528d28b3ac</t>
+  </si>
+  <si>
     <t xml:space="preserve">230e8d51-1f4d-3459-be47-429b0b828add</t>
   </si>
   <si>
     <t xml:space="preserve">fcdc8a7a-b10b-34bd-8ab3-65155dd4a762</t>
   </si>
   <si>
+    <t xml:space="preserve">a1baa4f2-50d3-44a1-b806-465c3d9ef1a7</t>
+  </si>
+  <si>
     <t xml:space="preserve">4edd87d7-666f-3226-a10c-a7b32d46f2fc</t>
   </si>
   <si>
+    <t xml:space="preserve">14712dc3-ca9f-4032-aed2-2e5f449c13cb</t>
+  </si>
+  <si>
     <t xml:space="preserve">88b44b36-2322-39a8-9c54-6b89b1b43cd4</t>
   </si>
   <si>
@@ -3407,34 +3431,58 @@
     <t xml:space="preserve">ce38752e-c414-3175-9482-ce663a909a0c</t>
   </si>
   <si>
+    <t xml:space="preserve">0704c700-2fb0-43c5-8803-bed8a6f1b968</t>
+  </si>
+  <si>
     <t xml:space="preserve">7b69255a-a7b2-318e-9433-54b7c4d13ece</t>
   </si>
   <si>
+    <t xml:space="preserve">84854d79-77da-4794-9d2a-f108f7e91741</t>
+  </si>
+  <si>
     <t xml:space="preserve">e10de570-42e6-3cb6-98fe-7bf6da57046c</t>
   </si>
   <si>
+    <t xml:space="preserve">db009019-338f-11dd-bd11-0800200c9a66</t>
+  </si>
+  <si>
     <t xml:space="preserve">0a075756-e4af-3da7-a521-c6f460e8470e</t>
   </si>
   <si>
+    <t xml:space="preserve">376c6e88-10e2-4acb-b676-6349cd260f3b</t>
+  </si>
+  <si>
     <t xml:space="preserve">b19fe3da-392e-36af-9342-910be1d2160a</t>
   </si>
   <si>
+    <t xml:space="preserve">ccbdee3b-27db-4852-a14c-ec73ad8421ea</t>
+  </si>
+  <si>
     <t xml:space="preserve">fa60e60f-73f0-3e20-bb3a-073e4a9469cc</t>
   </si>
   <si>
     <t xml:space="preserve">406f2854-27c5-3871-a9d5-80d29a4a39eb</t>
   </si>
   <si>
+    <t xml:space="preserve">e7920ba8-e048-49b5-b16b-387a937b901b</t>
+  </si>
+  <si>
     <t xml:space="preserve">a6cedcb1-f22c-3fc6-b6ee-7cb0c00da33d</t>
   </si>
   <si>
     <t xml:space="preserve">c378e883-97fc-3714-b923-d7271b8fcbac</t>
   </si>
   <si>
+    <t xml:space="preserve">119e8cc1-0859-45ca-8f63-93a8a518ffd2</t>
+  </si>
+  <si>
     <t xml:space="preserve">bc251c04-d2b2-366f-af0c-99d8fc2ed467</t>
   </si>
   <si>
     <t xml:space="preserve">7022c714-ec1a-3bec-ae9f-ed7769841d7c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9c0c2f04-fd6a-4d3c-950c-f9dead3639fe</t>
   </si>
   <si>
     <t xml:space="preserve">c19569ac-f0ab-453a-b70b-43f73bad11f8</t>
@@ -3562,7 +3610,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="1" sqref="D24 C2"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26014,7 +26062,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D24 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26073,15 +26121,16 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="37.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="61.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26120,6 +26169,9 @@
       <c r="E2" s="0" t="s">
         <v>1098</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>1099</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -26129,10 +26181,13 @@
         <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1100</v>
+        <v>1101</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>1102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26143,10 +26198,13 @@
         <v>49</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>1101</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>1100</v>
+      <c r="F4" s="0" t="s">
+        <v>1104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26157,10 +26215,13 @@
         <v>80</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>1103</v>
+        <v>1106</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26168,10 +26229,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26182,10 +26243,10 @@
         <v>52</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>1106</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26196,10 +26257,10 @@
         <v>337</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>1107</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26210,10 +26271,10 @@
         <v>850</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26224,10 +26285,13 @@
         <v>854</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>1109</v>
+        <v>1113</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>1114</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26238,10 +26302,13 @@
         <v>49</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>1110</v>
+        <v>1115</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>1097</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>1116</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26252,10 +26319,13 @@
         <v>49</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>1111</v>
+        <v>1117</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>1112</v>
+        <v>1118</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>1119</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26266,10 +26336,13 @@
         <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>1111</v>
+        <v>1117</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1113</v>
+        <v>1120</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26280,10 +26353,13 @@
         <v>80</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>1114</v>
+        <v>1122</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>1103</v>
+        <v>1106</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26294,10 +26370,13 @@
         <v>80</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>1114</v>
+        <v>1122</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>1103</v>
+        <v>1106</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26308,10 +26387,10 @@
         <v>37</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>1115</v>
+        <v>1123</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>1113</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26322,10 +26401,10 @@
         <v>260</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>1116</v>
+        <v>1124</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>1117</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26336,10 +26415,10 @@
         <v>285</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>1116</v>
+        <v>1124</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>1118</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26350,10 +26429,10 @@
         <v>294</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>1119</v>
+        <v>1127</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>1120</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26364,10 +26443,10 @@
         <v>302</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>1121</v>
+        <v>1129</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>1122</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26378,10 +26457,10 @@
         <v>328</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>1115</v>
+        <v>1123</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>1117</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26392,10 +26471,10 @@
         <v>349</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>1116</v>
+        <v>1124</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>1123</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26406,10 +26485,10 @@
         <v>357</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>1124</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26417,10 +26496,10 @@
         <v>36</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26431,10 +26510,10 @@
         <v>635</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>1124</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26445,10 +26524,10 @@
         <v>687</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>1123</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26459,10 +26538,10 @@
         <v>52</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>1106</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26473,10 +26552,10 @@
         <v>984</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>1116</v>
+        <v>1124</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>1118</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26487,10 +26566,13 @@
         <v>993</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>1124</v>
+        <v>1132</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>1114</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26501,10 +26583,13 @@
         <v>80</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>1111</v>
+        <v>1117</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>1103</v>
+        <v>1106</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26515,10 +26600,13 @@
         <v>20</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>1125</v>
+        <v>1133</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>1097</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>1134</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26529,10 +26617,13 @@
         <v>377</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>1126</v>
+        <v>1135</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>1120</v>
+        <v>1128</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>1136</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26543,10 +26634,13 @@
         <v>49</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>1127</v>
+        <v>1137</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>1097</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26554,10 +26648,13 @@
         <v>319</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>1127</v>
+        <v>1137</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>1097</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>1134</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26568,10 +26665,13 @@
         <v>49</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>1127</v>
+        <v>1137</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>1097</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>1136</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26582,10 +26682,13 @@
         <v>377</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>1127</v>
+        <v>1137</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>1120</v>
+        <v>1128</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>1136</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26596,10 +26699,13 @@
         <v>80</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>1127</v>
+        <v>1137</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>1097</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>1134</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26610,10 +26716,13 @@
         <v>49</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>1128</v>
+        <v>1139</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>1097</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>1140</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26624,10 +26733,13 @@
         <v>377</v>
       </c>
       <c r="C39" s="0" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>1128</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>1120</v>
+      <c r="F39" s="0" t="s">
+        <v>1140</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26638,10 +26750,13 @@
         <v>377</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>1129</v>
+        <v>1141</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>1120</v>
+        <v>1128</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>1142</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26652,10 +26767,13 @@
         <v>49</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>1130</v>
+        <v>1143</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>1131</v>
+        <v>1144</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>1145</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26666,10 +26784,13 @@
         <v>49</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>1130</v>
+        <v>1143</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>1132</v>
+        <v>1146</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>1145</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26680,10 +26801,13 @@
         <v>20</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>1133</v>
+        <v>1147</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>1113</v>
+        <v>1120</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26694,10 +26818,13 @@
         <v>49</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>1134</v>
+        <v>1149</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>1135</v>
+        <v>1150</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>1151</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26708,10 +26835,13 @@
         <v>49</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>1134</v>
+        <v>1149</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>1135</v>
+        <v>1150</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>1151</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26722,10 +26852,13 @@
         <v>80</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>1114</v>
+        <v>1122</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>1103</v>
+        <v>1106</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26736,10 +26869,13 @@
         <v>80</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>1114</v>
+        <v>1122</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>1103</v>
+        <v>1106</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26750,10 +26886,13 @@
         <v>20</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>1133</v>
+        <v>1147</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>1113</v>
+        <v>1120</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26764,10 +26903,13 @@
         <v>854</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>1109</v>
+        <v>1113</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>1114</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26778,10 +26920,13 @@
         <v>20</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>1113</v>
+        <v>1120</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26792,10 +26937,13 @@
         <v>80</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>1136</v>
+        <v>1152</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>1103</v>
+        <v>1106</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26806,10 +26954,13 @@
         <v>49</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>1137</v>
+        <v>1153</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>1135</v>
+        <v>1150</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>1151</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26820,10 +26971,13 @@
         <v>49</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>1138</v>
+        <v>1154</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>1119</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26834,10 +26988,13 @@
         <v>20</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>1139</v>
+        <v>1155</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>1113</v>
+        <v>1120</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>1121</v>
       </c>
     </row>
   </sheetData>
@@ -26859,20 +27016,20 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="D24 C27"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>1140</v>
+        <v>1156</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1141</v>
+        <v>1157</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1142</v>
+        <v>1158</v>
       </c>
       <c r="G1" s="1"/>
       <c r="I1" s="1"/>

</xml_diff>

<commit_message>
through PSM disclosures - descend / nondescend / mixed data
</commit_message>
<xml_diff>
--- a/jupyter/PSM-hackathon-leaf-flows_annotated.xlsx
+++ b/jupyter/PSM-hackathon-leaf-flows_annotated.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6414" uniqueCount="1159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6414" uniqueCount="1160">
   <si>
     <t xml:space="preserve">external_ref</t>
   </si>
@@ -3354,6 +3354,9 @@
   </si>
   <si>
     <t xml:space="preserve">076898a5-e1ce-3c50-9df4-6445fc0bb6aa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34e648e3-1797-3617-b316-64275060d73f</t>
   </si>
   <si>
     <t xml:space="preserve">49f5324b-fc33-36e9-b5af-3c80d73492bd</t>
@@ -26121,7 +26124,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26243,10 +26246,10 @@
         <v>52</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26260,7 +26263,7 @@
         <v>1108</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26285,13 +26288,13 @@
         <v>854</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26302,13 +26305,13 @@
         <v>49</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>1097</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26319,13 +26322,13 @@
         <v>49</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26336,13 +26339,13 @@
         <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26353,7 +26356,7 @@
         <v>80</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>1106</v>
@@ -26370,7 +26373,7 @@
         <v>80</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>1106</v>
@@ -26387,10 +26390,10 @@
         <v>37</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26401,10 +26404,10 @@
         <v>260</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26415,10 +26418,10 @@
         <v>285</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26429,10 +26432,10 @@
         <v>294</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26443,10 +26446,10 @@
         <v>302</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26457,10 +26460,10 @@
         <v>328</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26471,10 +26474,10 @@
         <v>349</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26488,7 +26491,7 @@
         <v>1108</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26513,7 +26516,7 @@
         <v>1108</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26527,7 +26530,7 @@
         <v>1108</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26538,10 +26541,10 @@
         <v>52</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26552,10 +26555,10 @@
         <v>984</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26566,13 +26569,13 @@
         <v>993</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26583,7 +26586,7 @@
         <v>80</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>1106</v>
@@ -26600,13 +26603,13 @@
         <v>20</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>1097</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26617,13 +26620,13 @@
         <v>377</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26634,13 +26637,13 @@
         <v>49</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>1097</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26648,13 +26651,13 @@
         <v>319</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>1097</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26665,13 +26668,13 @@
         <v>49</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>1097</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26682,13 +26685,13 @@
         <v>377</v>
       </c>
       <c r="C36" s="0" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F36" s="0" t="s">
         <v>1137</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>1128</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>1136</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26699,13 +26702,13 @@
         <v>80</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>1097</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26716,13 +26719,13 @@
         <v>49</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>1097</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26733,13 +26736,13 @@
         <v>377</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26750,13 +26753,13 @@
         <v>377</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26767,13 +26770,13 @@
         <v>49</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26784,13 +26787,13 @@
         <v>49</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="D42" s="0" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F42" s="0" t="s">
         <v>1146</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26801,13 +26804,13 @@
         <v>20</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26818,13 +26821,13 @@
         <v>49</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26835,13 +26838,13 @@
         <v>49</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26852,7 +26855,7 @@
         <v>80</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>1106</v>
@@ -26869,7 +26872,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>1106</v>
@@ -26886,13 +26889,13 @@
         <v>20</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26903,13 +26906,13 @@
         <v>854</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26920,13 +26923,13 @@
         <v>20</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26937,7 +26940,7 @@
         <v>80</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>1106</v>
@@ -26954,13 +26957,13 @@
         <v>49</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26974,10 +26977,10 @@
         <v>1103</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26988,13 +26991,13 @@
         <v>20</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
     </row>
   </sheetData>
@@ -27023,13 +27026,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="G1" s="1"/>
       <c r="I1" s="1"/>

</xml_diff>